<commit_message>
Case 3 with daily snow depth and reduced snow density - work on processing the datasets
</commit_message>
<xml_diff>
--- a/9_article1_FigsTables_ces/Tables_data/res_mean_std.xlsx
+++ b/9_article1_FigsTables_ces/Tables_data/res_mean_std.xlsx
@@ -451,16 +451,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.121</v>
+        <v>0.573</v>
       </c>
       <c r="C4">
-        <v>4.408</v>
+        <v>2.108</v>
       </c>
       <c r="D4">
-        <v>6.291</v>
+        <v>1.781</v>
       </c>
       <c r="E4">
-        <v>10.914</v>
+        <v>5.581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>